<commit_message>
update raw result with c = 0.1 with sigmiod kernel
</commit_message>
<xml_diff>
--- a/EDA_Process/C_Morlet_SVM/SVM_raw_result_33.xlsx
+++ b/EDA_Process/C_Morlet_SVM/SVM_raw_result_33.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fengh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LabWork\ThesisProject\Music_Autism_Robot\EDA_Process\C_Morlet_SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A2F286-DAC4-4F17-A1FC-2A595F3D6EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9B4240-6582-4F3E-A1A3-6344469D2F3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="81">
   <si>
     <t>Linear</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>SVMAccuracy: 33.3333</t>
+  </si>
+  <si>
+    <t>SVMAccuracy : 60.6061</t>
+  </si>
+  <si>
+    <t>21  48  30</t>
+  </si>
+  <si>
+    <t>42  42  15</t>
+  </si>
+  <si>
+    <t>24  36  39</t>
   </si>
 </sst>
 </file>
@@ -573,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -584,6 +596,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="19.87890625" customWidth="1"/>
     <col min="4" max="4" width="19.5859375" customWidth="1"/>
+    <col min="5" max="5" width="19.9375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
@@ -725,7 +738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -736,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -747,12 +760,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -763,7 +776,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -774,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
         <v>37</v>
       </c>
@@ -785,7 +798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
         <v>38</v>
       </c>
@@ -796,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -807,7 +820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -815,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
         <v>40</v>
       </c>
@@ -825,8 +838,11 @@
       <c r="D28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -836,8 +852,11 @@
       <c r="D29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -847,8 +866,11 @@
       <c r="D30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -858,13 +880,16 @@
       <c r="D31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
         <v>21</v>
       </c>
@@ -874,8 +899,11 @@
       <c r="D34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -885,8 +913,11 @@
       <c r="D35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -896,8 +927,11 @@
       <c r="D36" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B37" t="s">
         <v>18</v>
       </c>
@@ -907,13 +941,16 @@
       <c r="D37" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B40" t="s">
         <v>15</v>
       </c>
@@ -923,8 +960,11 @@
       <c r="D40" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -934,8 +974,11 @@
       <c r="D41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -945,8 +988,11 @@
       <c r="D42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
         <v>18</v>
       </c>
@@ -956,13 +1002,16 @@
       <c r="D43" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B46" t="s">
         <v>36</v>
       </c>
@@ -972,8 +1021,11 @@
       <c r="D46" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B47" t="s">
         <v>6</v>
       </c>
@@ -983,8 +1035,11 @@
       <c r="D47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
         <v>48</v>
       </c>
@@ -994,8 +1049,11 @@
       <c r="D48" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
         <v>49</v>
       </c>
@@ -1005,8 +1063,11 @@
       <c r="D49" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B50" t="s">
         <v>50</v>
       </c>
@@ -1016,8 +1077,11 @@
       <c r="D50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -1025,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B53" t="s">
         <v>45</v>
       </c>
@@ -1036,7 +1100,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B54" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B55" t="s">
         <v>41</v>
       </c>
@@ -1058,7 +1122,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
         <v>25</v>
       </c>
@@ -1069,12 +1133,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B58" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B59" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1149,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B60" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B61" t="s">
         <v>42</v>
       </c>
@@ -1107,7 +1171,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B62" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B64" t="s">
         <v>13</v>
       </c>

</xml_diff>